<commit_message>
credit_score addition + results
</commit_message>
<xml_diff>
--- a/results/final_results.xlsx
+++ b/results/final_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omerh\PycharmProjects\Thesis\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64169A3-7A4F-487B-AA74-9376C67950BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE73571E-2E28-48C8-A661-F8A118D321DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2BBAB6F4-6D61-40AD-8AC7-5B9147BF3A32}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>date</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>mean</t>
+  </si>
+  <si>
+    <t>default + 0 heuristic</t>
   </si>
 </sst>
 </file>
@@ -247,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -261,6 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42ED80D-E974-414B-A344-D70D318FFA08}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E20" workbookViewId="0">
-      <selection activeCell="Q30" sqref="Q1:R30"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -598,9 +602,10 @@
     <col min="15" max="16" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.36328125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,8 +660,11 @@
       <c r="R1" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S1" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44967</v>
       </c>
@@ -715,8 +723,12 @@
         <f>IF(P2&gt;N2, 1, 0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S2">
+        <f>IF(J2&gt;N2, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44967</v>
       </c>
@@ -775,8 +787,12 @@
         <f t="shared" ref="R3:R30" si="3">IF(P3&gt;N3, 1, 0)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S3">
+        <f t="shared" ref="S3:S31" si="4">IF(J3&gt;N3, 1, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44967</v>
       </c>
@@ -835,8 +851,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S4">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44967</v>
       </c>
@@ -895,8 +915,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44967</v>
       </c>
@@ -955,8 +979,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S6">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44967</v>
       </c>
@@ -1015,8 +1043,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S7">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44967</v>
       </c>
@@ -1075,8 +1107,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44967</v>
       </c>
@@ -1135,8 +1171,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>44967</v>
       </c>
@@ -1195,8 +1235,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44967</v>
       </c>
@@ -1255,8 +1299,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44967</v>
       </c>
@@ -1315,8 +1363,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S12">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44967</v>
       </c>
@@ -1375,8 +1427,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44967</v>
       </c>
@@ -1435,8 +1491,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S14">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44967</v>
       </c>
@@ -1495,8 +1555,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S15">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>44967</v>
       </c>
@@ -1555,8 +1619,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S16">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>44967</v>
       </c>
@@ -1615,8 +1683,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S17">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>44967</v>
       </c>
@@ -1675,8 +1747,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S18">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>44967</v>
       </c>
@@ -1735,8 +1811,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>44967</v>
       </c>
@@ -1795,8 +1875,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>44967</v>
       </c>
@@ -1855,8 +1939,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S21">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>44967</v>
       </c>
@@ -1915,8 +2003,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>44967</v>
       </c>
@@ -1975,8 +2067,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>44967</v>
       </c>
@@ -2035,8 +2131,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>44967</v>
       </c>
@@ -2095,8 +2195,12 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>44967</v>
       </c>
@@ -2155,8 +2259,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>44967</v>
       </c>
@@ -2215,8 +2323,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>44967</v>
       </c>
@@ -2275,8 +2387,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="S28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>44967</v>
       </c>
@@ -2335,8 +2451,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="2">
         <v>44967</v>
       </c>
@@ -2395,8 +2515,12 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="S30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="P31" s="8" t="s">
         <v>23</v>
       </c>
@@ -2407,6 +2531,24 @@
       <c r="R31" s="12">
         <f>AVERAGE(R2:R30)</f>
         <v>0.72413793103448276</v>
+      </c>
+      <c r="S31" s="12">
+        <f>AVERAGE(S2:S30)</f>
+        <v>0.27586206896551724</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="Q32" s="13">
+        <f>AVERAGE(Q2:Q24)</f>
+        <v>0.47826086956521741</v>
+      </c>
+      <c r="R32" s="13">
+        <f>AVERAGE(R2:R24)</f>
+        <v>0.86956521739130432</v>
+      </c>
+      <c r="S32" s="13">
+        <f>AVERAGE(S2:S24)</f>
+        <v>0.34782608695652173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>